<commit_message>
fix crec - all those fields are not needed
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -1,46 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E027565-0898-EC48-9542-5DD2180223C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="crec_persons" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="crec_lookup" sheetId="2" r:id="rId5"/>
+    <sheet name="crec_persons" sheetId="1" r:id="rId1"/>
+    <sheet name="crec_lookup" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">crec_persons!$A$1:$P$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crec_persons!$A$1:$P$82</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="I5">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <t xml:space="preserve">added col name
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>added col name
 	-Jennifer Mackown</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="J5">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <t xml:space="preserve">removed "no", not required
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>removed "no", not required
 	-Jennifer Mackown</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="J9">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <t xml:space="preserve">removed "unknown"
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>removed "unknown"
 	-Jennifer Mackown</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="J17">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
-        <t xml:space="preserve">removed 'unique_number' - makes more sense as a calculation than a transformation
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>removed 'unique_number' - makes more sense as a calculation than a transformation
 	-Jennifer Mackown</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -48,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="116">
   <si>
     <t>table_name</t>
   </si>
@@ -419,51 +457,54 @@
   <si>
     <t>null</t>
   </si>
+  <si>
+    <t>not mapped</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -473,7 +514,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -489,7 +530,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -503,8 +550,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -514,86 +563,71 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -783,40 +817,42 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
-    <col customWidth="1" min="2" max="2" width="26.29"/>
-    <col customWidth="1" min="3" max="3" width="12.86"/>
-    <col customWidth="1" hidden="1" min="4" max="4" width="16.57"/>
-    <col customWidth="1" hidden="1" min="5" max="5" width="41.29"/>
-    <col customWidth="1" min="6" max="6" width="16.14"/>
-    <col customWidth="1" min="7" max="7" width="14.86"/>
-    <col customWidth="1" min="8" max="8" width="22.86"/>
-    <col customWidth="1" min="9" max="9" width="23.57"/>
-    <col customWidth="1" min="10" max="10" width="25.29"/>
-    <col customWidth="1" min="11" max="11" width="29.29"/>
-    <col customWidth="1" min="12" max="12" width="17.86"/>
-    <col customWidth="1" min="13" max="15" width="14.43"/>
-    <col customWidth="1" min="16" max="16" width="56.71"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="13" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.0" customHeight="1">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -891,10 +927,12 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -917,10 +955,12 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="O3" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P3" s="4"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -943,10 +983,12 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P4" s="4"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -969,10 +1011,12 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P5" s="4"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -995,10 +1039,12 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="O6" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P6" s="4"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1021,10 +1067,12 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1047,10 +1095,12 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1073,10 +1123,12 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1099,10 +1151,12 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="O10" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1125,10 +1179,12 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="O11" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1151,10 +1207,12 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="O12" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1177,10 +1235,12 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="O13" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1203,10 +1263,12 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="O14" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1229,10 +1291,12 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="O15" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1255,10 +1319,12 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="O16" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1281,10 +1347,12 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="O17" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1307,10 +1375,12 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="O18" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1333,10 +1403,12 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="O19" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1359,10 +1431,12 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="O20" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1385,10 +1459,12 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+      <c r="O21" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -1411,10 +1487,12 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
+      <c r="O22" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1437,10 +1515,12 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="O23" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -1463,10 +1543,12 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
+      <c r="O24" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1489,10 +1571,12 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
+      <c r="O25" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1515,10 +1599,12 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="O26" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -1541,10 +1627,12 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
+      <c r="O27" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -1567,10 +1655,12 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
+      <c r="O28" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1593,10 +1683,12 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
+      <c r="O29" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -1619,10 +1711,12 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
+      <c r="O30" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P30" s="4"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -1645,10 +1739,12 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
+      <c r="O31" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -1671,10 +1767,12 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
+      <c r="O32" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -1697,10 +1795,12 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
+      <c r="O33" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -1723,10 +1823,12 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
+      <c r="O34" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -1749,10 +1851,12 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
+      <c r="O35" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P35" s="4"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -1775,10 +1879,12 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
+      <c r="O36" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P36" s="4"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -1801,10 +1907,12 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
+      <c r="O37" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P37" s="4"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1827,10 +1935,12 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
+      <c r="O38" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P38" s="4"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
@@ -1853,10 +1963,12 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
+      <c r="O39" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P39" s="4"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
@@ -1879,10 +1991,12 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
+      <c r="O40" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P40" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -1905,10 +2019,12 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
+      <c r="O41" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P41" s="4"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
@@ -1931,10 +2047,12 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
+      <c r="O42" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P42" s="4"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -1957,10 +2075,12 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
+      <c r="O43" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P43" s="4"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>16</v>
       </c>
@@ -1983,10 +2103,12 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
+      <c r="O44" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P44" s="4"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>16</v>
       </c>
@@ -2009,10 +2131,12 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
+      <c r="O45" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P45" s="4"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>16</v>
       </c>
@@ -2035,10 +2159,12 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
+      <c r="O46" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
@@ -2061,10 +2187,12 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
+      <c r="O47" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P47" s="4"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>16</v>
       </c>
@@ -2087,10 +2215,12 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
+      <c r="O48" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P48" s="4"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -2113,10 +2243,12 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
+      <c r="O49" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P49" s="4"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -2129,7 +2261,8 @@
       <c r="D50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="19"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -2138,10 +2271,12 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
+      <c r="O50" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P50" s="4"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
@@ -2164,10 +2299,12 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
+      <c r="O51" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P51" s="4"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>16</v>
       </c>
@@ -2180,7 +2317,8 @@
       <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -2189,10 +2327,12 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
+      <c r="O52" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P52" s="4"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>16</v>
       </c>
@@ -2215,10 +2355,12 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
+      <c r="O53" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P53" s="4"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>16</v>
       </c>
@@ -2241,10 +2383,12 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
+      <c r="O54" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P54" s="4"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>16</v>
       </c>
@@ -2267,10 +2411,12 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
+      <c r="O55" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P55" s="4"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>16</v>
       </c>
@@ -2293,10 +2439,12 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
+      <c r="O56" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P56" s="4"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>16</v>
       </c>
@@ -2319,10 +2467,12 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
+      <c r="O57" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P57" s="4"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>16</v>
       </c>
@@ -2345,10 +2495,12 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
+      <c r="O58" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P58" s="4"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>16</v>
       </c>
@@ -2371,10 +2523,12 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
+      <c r="O59" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P59" s="4"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>16</v>
       </c>
@@ -2397,10 +2551,12 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
+      <c r="O60" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P60" s="4"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
@@ -2423,10 +2579,12 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
+      <c r="O61" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P61" s="4"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>16</v>
       </c>
@@ -2449,10 +2607,12 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
+      <c r="O62" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P62" s="4"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>16</v>
       </c>
@@ -2475,10 +2635,12 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
+      <c r="O63" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P63" s="4"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>16</v>
       </c>
@@ -2501,10 +2663,12 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
+      <c r="O64" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P64" s="4"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>16</v>
       </c>
@@ -2527,10 +2691,12 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
+      <c r="O65" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P65" s="4"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>16</v>
       </c>
@@ -2553,10 +2719,12 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
+      <c r="O66" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P66" s="4"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>16</v>
       </c>
@@ -2579,10 +2747,12 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
+      <c r="O67" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P67" s="4"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>16</v>
       </c>
@@ -2605,10 +2775,12 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
+      <c r="O68" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P68" s="4"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>16</v>
       </c>
@@ -2631,10 +2803,12 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
+      <c r="O69" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P69" s="4"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>16</v>
       </c>
@@ -2657,10 +2831,12 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
+      <c r="O70" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P70" s="4"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>16</v>
       </c>
@@ -2683,10 +2859,12 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
+      <c r="O71" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P71" s="4"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>16</v>
       </c>
@@ -2709,10 +2887,12 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
+      <c r="O72" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P72" s="4"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>16</v>
       </c>
@@ -2735,10 +2915,12 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
+      <c r="O73" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P73" s="4"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>16</v>
       </c>
@@ -2761,10 +2943,12 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
+      <c r="O74" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P74" s="4"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>16</v>
       </c>
@@ -2777,7 +2961,8 @@
       <c r="D75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E75" s="4"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="19"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -2786,10 +2971,12 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
+      <c r="O75" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P75" s="4"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>16</v>
       </c>
@@ -2814,10 +3001,12 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
+      <c r="O76" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P76" s="4"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>16</v>
       </c>
@@ -2830,7 +3019,8 @@
       <c r="D77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E77" s="4"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="19"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -2839,10 +3029,12 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
+      <c r="O77" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P77" s="4"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>16</v>
       </c>
@@ -2865,10 +3057,12 @@
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
+      <c r="O78" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P78" s="4"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>16</v>
       </c>
@@ -2902,7 +3096,7 @@
       </c>
       <c r="P79" s="4"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>16</v>
       </c>
@@ -2915,7 +3109,8 @@
       <c r="D80" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E80" s="4"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="19"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
@@ -2924,10 +3119,12 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
+      <c r="O80" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P80" s="4"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
@@ -2950,10 +3147,12 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
+      <c r="O81" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P81" s="4"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>16</v>
       </c>
@@ -2976,929 +3175,931 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
+      <c r="O82" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="P82" s="4"/>
     </row>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
-    <row r="201"/>
-    <row r="202"/>
-    <row r="203"/>
-    <row r="204"/>
-    <row r="205"/>
-    <row r="206"/>
-    <row r="207"/>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212"/>
-    <row r="213"/>
-    <row r="214"/>
-    <row r="215"/>
-    <row r="216"/>
-    <row r="217"/>
-    <row r="218"/>
-    <row r="219"/>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
-    <row r="224"/>
-    <row r="225"/>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230"/>
-    <row r="231"/>
-    <row r="232"/>
-    <row r="233"/>
-    <row r="234"/>
-    <row r="235"/>
-    <row r="236"/>
-    <row r="237"/>
-    <row r="238"/>
-    <row r="239"/>
-    <row r="240"/>
-    <row r="241"/>
-    <row r="242"/>
-    <row r="243"/>
-    <row r="244"/>
-    <row r="245"/>
-    <row r="246"/>
-    <row r="247"/>
-    <row r="248"/>
-    <row r="249"/>
-    <row r="250"/>
-    <row r="251"/>
-    <row r="252"/>
-    <row r="253"/>
-    <row r="254"/>
-    <row r="255"/>
-    <row r="256"/>
-    <row r="257"/>
-    <row r="258"/>
-    <row r="259"/>
-    <row r="260"/>
-    <row r="261"/>
-    <row r="262"/>
-    <row r="263"/>
-    <row r="264"/>
-    <row r="265"/>
-    <row r="266"/>
-    <row r="267"/>
-    <row r="268"/>
-    <row r="269"/>
-    <row r="270"/>
-    <row r="271"/>
-    <row r="272"/>
-    <row r="273"/>
-    <row r="274"/>
-    <row r="275"/>
-    <row r="276"/>
-    <row r="277"/>
-    <row r="278"/>
-    <row r="279"/>
-    <row r="280"/>
-    <row r="281"/>
-    <row r="282"/>
-    <row r="283"/>
-    <row r="284"/>
-    <row r="285"/>
-    <row r="286"/>
-    <row r="287"/>
-    <row r="288"/>
-    <row r="289"/>
-    <row r="290"/>
-    <row r="291"/>
-    <row r="292"/>
-    <row r="293"/>
-    <row r="294"/>
-    <row r="295"/>
-    <row r="296"/>
-    <row r="297"/>
-    <row r="298"/>
-    <row r="299"/>
-    <row r="300"/>
-    <row r="301"/>
-    <row r="302"/>
-    <row r="303"/>
-    <row r="304"/>
-    <row r="305"/>
-    <row r="306"/>
-    <row r="307"/>
-    <row r="308"/>
-    <row r="309"/>
-    <row r="310"/>
-    <row r="311"/>
-    <row r="312"/>
-    <row r="313"/>
-    <row r="314"/>
-    <row r="315"/>
-    <row r="316"/>
-    <row r="317"/>
-    <row r="318"/>
-    <row r="319"/>
-    <row r="320"/>
-    <row r="321"/>
-    <row r="322"/>
-    <row r="323"/>
-    <row r="324"/>
-    <row r="325"/>
-    <row r="326"/>
-    <row r="327"/>
-    <row r="328"/>
-    <row r="329"/>
-    <row r="330"/>
-    <row r="331"/>
-    <row r="332"/>
-    <row r="333"/>
-    <row r="334"/>
-    <row r="335"/>
-    <row r="336"/>
-    <row r="337"/>
-    <row r="338"/>
-    <row r="339"/>
-    <row r="340"/>
-    <row r="341"/>
-    <row r="342"/>
-    <row r="343"/>
-    <row r="344"/>
-    <row r="345"/>
-    <row r="346"/>
-    <row r="347"/>
-    <row r="348"/>
-    <row r="349"/>
-    <row r="350"/>
-    <row r="351"/>
-    <row r="352"/>
-    <row r="353"/>
-    <row r="354"/>
-    <row r="355"/>
-    <row r="356"/>
-    <row r="357"/>
-    <row r="358"/>
-    <row r="359"/>
-    <row r="360"/>
-    <row r="361"/>
-    <row r="362"/>
-    <row r="363"/>
-    <row r="364"/>
-    <row r="365"/>
-    <row r="366"/>
-    <row r="367"/>
-    <row r="368"/>
-    <row r="369"/>
-    <row r="370"/>
-    <row r="371"/>
-    <row r="372"/>
-    <row r="373"/>
-    <row r="374"/>
-    <row r="375"/>
-    <row r="376"/>
-    <row r="377"/>
-    <row r="378"/>
-    <row r="379"/>
-    <row r="380"/>
-    <row r="381"/>
-    <row r="382"/>
-    <row r="383"/>
-    <row r="384"/>
-    <row r="385"/>
-    <row r="386"/>
-    <row r="387"/>
-    <row r="388"/>
-    <row r="389"/>
-    <row r="390"/>
-    <row r="391"/>
-    <row r="392"/>
-    <row r="393"/>
-    <row r="394"/>
-    <row r="395"/>
-    <row r="396"/>
-    <row r="397"/>
-    <row r="398"/>
-    <row r="399"/>
-    <row r="400"/>
-    <row r="401"/>
-    <row r="402"/>
-    <row r="403"/>
-    <row r="404"/>
-    <row r="405"/>
-    <row r="406"/>
-    <row r="407"/>
-    <row r="408"/>
-    <row r="409"/>
-    <row r="410"/>
-    <row r="411"/>
-    <row r="412"/>
-    <row r="413"/>
-    <row r="414"/>
-    <row r="415"/>
-    <row r="416"/>
-    <row r="417"/>
-    <row r="418"/>
-    <row r="419"/>
-    <row r="420"/>
-    <row r="421"/>
-    <row r="422"/>
-    <row r="423"/>
-    <row r="424"/>
-    <row r="425"/>
-    <row r="426"/>
-    <row r="427"/>
-    <row r="428"/>
-    <row r="429"/>
-    <row r="430"/>
-    <row r="431"/>
-    <row r="432"/>
-    <row r="433"/>
-    <row r="434"/>
-    <row r="435"/>
-    <row r="436"/>
-    <row r="437"/>
-    <row r="438"/>
-    <row r="439"/>
-    <row r="440"/>
-    <row r="441"/>
-    <row r="442"/>
-    <row r="443"/>
-    <row r="444"/>
-    <row r="445"/>
-    <row r="446"/>
-    <row r="447"/>
-    <row r="448"/>
-    <row r="449"/>
-    <row r="450"/>
-    <row r="451"/>
-    <row r="452"/>
-    <row r="453"/>
-    <row r="454"/>
-    <row r="455"/>
-    <row r="456"/>
-    <row r="457"/>
-    <row r="458"/>
-    <row r="459"/>
-    <row r="460"/>
-    <row r="461"/>
-    <row r="462"/>
-    <row r="463"/>
-    <row r="464"/>
-    <row r="465"/>
-    <row r="466"/>
-    <row r="467"/>
-    <row r="468"/>
-    <row r="469"/>
-    <row r="470"/>
-    <row r="471"/>
-    <row r="472"/>
-    <row r="473"/>
-    <row r="474"/>
-    <row r="475"/>
-    <row r="476"/>
-    <row r="477"/>
-    <row r="478"/>
-    <row r="479"/>
-    <row r="480"/>
-    <row r="481"/>
-    <row r="482"/>
-    <row r="483"/>
-    <row r="484"/>
-    <row r="485"/>
-    <row r="486"/>
-    <row r="487"/>
-    <row r="488"/>
-    <row r="489"/>
-    <row r="490"/>
-    <row r="491"/>
-    <row r="492"/>
-    <row r="493"/>
-    <row r="494"/>
-    <row r="495"/>
-    <row r="496"/>
-    <row r="497"/>
-    <row r="498"/>
-    <row r="499"/>
-    <row r="500"/>
-    <row r="501"/>
-    <row r="502"/>
-    <row r="503"/>
-    <row r="504"/>
-    <row r="505"/>
-    <row r="506"/>
-    <row r="507"/>
-    <row r="508"/>
-    <row r="509"/>
-    <row r="510"/>
-    <row r="511"/>
-    <row r="512"/>
-    <row r="513"/>
-    <row r="514"/>
-    <row r="515"/>
-    <row r="516"/>
-    <row r="517"/>
-    <row r="518"/>
-    <row r="519"/>
-    <row r="520"/>
-    <row r="521"/>
-    <row r="522"/>
-    <row r="523"/>
-    <row r="524"/>
-    <row r="525"/>
-    <row r="526"/>
-    <row r="527"/>
-    <row r="528"/>
-    <row r="529"/>
-    <row r="530"/>
-    <row r="531"/>
-    <row r="532"/>
-    <row r="533"/>
-    <row r="534"/>
-    <row r="535"/>
-    <row r="536"/>
-    <row r="537"/>
-    <row r="538"/>
-    <row r="539"/>
-    <row r="540"/>
-    <row r="541"/>
-    <row r="542"/>
-    <row r="543"/>
-    <row r="544"/>
-    <row r="545"/>
-    <row r="546"/>
-    <row r="547"/>
-    <row r="548"/>
-    <row r="549"/>
-    <row r="550"/>
-    <row r="551"/>
-    <row r="552"/>
-    <row r="553"/>
-    <row r="554"/>
-    <row r="555"/>
-    <row r="556"/>
-    <row r="557"/>
-    <row r="558"/>
-    <row r="559"/>
-    <row r="560"/>
-    <row r="561"/>
-    <row r="562"/>
-    <row r="563"/>
-    <row r="564"/>
-    <row r="565"/>
-    <row r="566"/>
-    <row r="567"/>
-    <row r="568"/>
-    <row r="569"/>
-    <row r="570"/>
-    <row r="571"/>
-    <row r="572"/>
-    <row r="573"/>
-    <row r="574"/>
-    <row r="575"/>
-    <row r="576"/>
-    <row r="577"/>
-    <row r="578"/>
-    <row r="579"/>
-    <row r="580"/>
-    <row r="581"/>
-    <row r="582"/>
-    <row r="583"/>
-    <row r="584"/>
-    <row r="585"/>
-    <row r="586"/>
-    <row r="587"/>
-    <row r="588"/>
-    <row r="589"/>
-    <row r="590"/>
-    <row r="591"/>
-    <row r="592"/>
-    <row r="593"/>
-    <row r="594"/>
-    <row r="595"/>
-    <row r="596"/>
-    <row r="597"/>
-    <row r="598"/>
-    <row r="599"/>
-    <row r="600"/>
-    <row r="601"/>
-    <row r="602"/>
-    <row r="603"/>
-    <row r="604"/>
-    <row r="605"/>
-    <row r="606"/>
-    <row r="607"/>
-    <row r="608"/>
-    <row r="609"/>
-    <row r="610"/>
-    <row r="611"/>
-    <row r="612"/>
-    <row r="613"/>
-    <row r="614"/>
-    <row r="615"/>
-    <row r="616"/>
-    <row r="617"/>
-    <row r="618"/>
-    <row r="619"/>
-    <row r="620"/>
-    <row r="621"/>
-    <row r="622"/>
-    <row r="623"/>
-    <row r="624"/>
-    <row r="625"/>
-    <row r="626"/>
-    <row r="627"/>
-    <row r="628"/>
-    <row r="629"/>
-    <row r="630"/>
-    <row r="631"/>
-    <row r="632"/>
-    <row r="633"/>
-    <row r="634"/>
-    <row r="635"/>
-    <row r="636"/>
-    <row r="637"/>
-    <row r="638"/>
-    <row r="639"/>
-    <row r="640"/>
-    <row r="641"/>
-    <row r="642"/>
-    <row r="643"/>
-    <row r="644"/>
-    <row r="645"/>
-    <row r="646"/>
-    <row r="647"/>
-    <row r="648"/>
-    <row r="649"/>
-    <row r="650"/>
-    <row r="651"/>
-    <row r="652"/>
-    <row r="653"/>
-    <row r="654"/>
-    <row r="655"/>
-    <row r="656"/>
-    <row r="657"/>
-    <row r="658"/>
-    <row r="659"/>
-    <row r="660"/>
-    <row r="661"/>
-    <row r="662"/>
-    <row r="663"/>
-    <row r="664"/>
-    <row r="665"/>
-    <row r="666"/>
-    <row r="667"/>
-    <row r="668"/>
-    <row r="669"/>
-    <row r="670"/>
-    <row r="671"/>
-    <row r="672"/>
-    <row r="673"/>
-    <row r="674"/>
-    <row r="675"/>
-    <row r="676"/>
-    <row r="677"/>
-    <row r="678"/>
-    <row r="679"/>
-    <row r="680"/>
-    <row r="681"/>
-    <row r="682"/>
-    <row r="683"/>
-    <row r="684"/>
-    <row r="685"/>
-    <row r="686"/>
-    <row r="687"/>
-    <row r="688"/>
-    <row r="689"/>
-    <row r="690"/>
-    <row r="691"/>
-    <row r="692"/>
-    <row r="693"/>
-    <row r="694"/>
-    <row r="695"/>
-    <row r="696"/>
-    <row r="697"/>
-    <row r="698"/>
-    <row r="699"/>
-    <row r="700"/>
-    <row r="701"/>
-    <row r="702"/>
-    <row r="703"/>
-    <row r="704"/>
-    <row r="705"/>
-    <row r="706"/>
-    <row r="707"/>
-    <row r="708"/>
-    <row r="709"/>
-    <row r="710"/>
-    <row r="711"/>
-    <row r="712"/>
-    <row r="713"/>
-    <row r="714"/>
-    <row r="715"/>
-    <row r="716"/>
-    <row r="717"/>
-    <row r="718"/>
-    <row r="719"/>
-    <row r="720"/>
-    <row r="721"/>
-    <row r="722"/>
-    <row r="723"/>
-    <row r="724"/>
-    <row r="725"/>
-    <row r="726"/>
-    <row r="727"/>
-    <row r="728"/>
-    <row r="729"/>
-    <row r="730"/>
-    <row r="731"/>
-    <row r="732"/>
-    <row r="733"/>
-    <row r="734"/>
-    <row r="735"/>
-    <row r="736"/>
-    <row r="737"/>
-    <row r="738"/>
-    <row r="739"/>
-    <row r="740"/>
-    <row r="741"/>
-    <row r="742"/>
-    <row r="743"/>
-    <row r="744"/>
-    <row r="745"/>
-    <row r="746"/>
-    <row r="747"/>
-    <row r="748"/>
-    <row r="749"/>
-    <row r="750"/>
-    <row r="751"/>
-    <row r="752"/>
-    <row r="753"/>
-    <row r="754"/>
-    <row r="755"/>
-    <row r="756"/>
-    <row r="757"/>
-    <row r="758"/>
-    <row r="759"/>
-    <row r="760"/>
-    <row r="761"/>
-    <row r="762"/>
-    <row r="763"/>
-    <row r="764"/>
-    <row r="765"/>
-    <row r="766"/>
-    <row r="767"/>
-    <row r="768"/>
-    <row r="769"/>
-    <row r="770"/>
-    <row r="771"/>
-    <row r="772"/>
-    <row r="773"/>
-    <row r="774"/>
-    <row r="775"/>
-    <row r="776"/>
-    <row r="777"/>
-    <row r="778"/>
-    <row r="779"/>
-    <row r="780"/>
-    <row r="781"/>
-    <row r="782"/>
-    <row r="783"/>
-    <row r="784"/>
-    <row r="785"/>
-    <row r="786"/>
-    <row r="787"/>
-    <row r="788"/>
-    <row r="789"/>
-    <row r="790"/>
-    <row r="791"/>
-    <row r="792"/>
-    <row r="793"/>
-    <row r="794"/>
-    <row r="795"/>
-    <row r="796"/>
-    <row r="797"/>
-    <row r="798"/>
-    <row r="799"/>
-    <row r="800"/>
-    <row r="801"/>
-    <row r="802"/>
-    <row r="803"/>
-    <row r="804"/>
-    <row r="805"/>
-    <row r="806"/>
-    <row r="807"/>
-    <row r="808"/>
-    <row r="809"/>
-    <row r="810"/>
-    <row r="811"/>
-    <row r="812"/>
-    <row r="813"/>
-    <row r="814"/>
-    <row r="815"/>
-    <row r="816"/>
-    <row r="817"/>
-    <row r="818"/>
-    <row r="819"/>
-    <row r="820"/>
-    <row r="821"/>
-    <row r="822"/>
-    <row r="823"/>
-    <row r="824"/>
-    <row r="825"/>
-    <row r="826"/>
-    <row r="827"/>
-    <row r="828"/>
-    <row r="829"/>
-    <row r="830"/>
-    <row r="831"/>
-    <row r="832"/>
-    <row r="833"/>
-    <row r="834"/>
-    <row r="835"/>
-    <row r="836"/>
-    <row r="837"/>
-    <row r="838"/>
-    <row r="839"/>
-    <row r="840"/>
-    <row r="841"/>
-    <row r="842"/>
-    <row r="843"/>
-    <row r="844"/>
-    <row r="845"/>
-    <row r="846"/>
-    <row r="847"/>
-    <row r="848"/>
-    <row r="849"/>
-    <row r="850"/>
-    <row r="851"/>
-    <row r="852"/>
-    <row r="853"/>
-    <row r="854"/>
-    <row r="855"/>
-    <row r="856"/>
-    <row r="857"/>
-    <row r="858"/>
-    <row r="859"/>
-    <row r="860"/>
-    <row r="861"/>
-    <row r="862"/>
-    <row r="863"/>
-    <row r="864"/>
-    <row r="865"/>
-    <row r="866"/>
-    <row r="867"/>
-    <row r="868"/>
-    <row r="869"/>
-    <row r="870"/>
-    <row r="871"/>
-    <row r="872"/>
-    <row r="873"/>
-    <row r="874"/>
-    <row r="875"/>
-    <row r="876"/>
-    <row r="877"/>
-    <row r="878"/>
-    <row r="879"/>
-    <row r="880"/>
-    <row r="881"/>
-    <row r="882"/>
-    <row r="883"/>
-    <row r="884"/>
-    <row r="885"/>
-    <row r="886"/>
-    <row r="887"/>
-    <row r="888"/>
-    <row r="889"/>
-    <row r="890"/>
-    <row r="891"/>
-    <row r="892"/>
-    <row r="893"/>
-    <row r="894"/>
-    <row r="895"/>
-    <row r="896"/>
-    <row r="897"/>
-    <row r="898"/>
-    <row r="899"/>
-    <row r="900"/>
-    <row r="901"/>
-    <row r="902"/>
-    <row r="903"/>
-    <row r="904"/>
-    <row r="905"/>
-    <row r="906"/>
-    <row r="907"/>
-    <row r="908"/>
-    <row r="909"/>
-    <row r="910"/>
-    <row r="911"/>
-    <row r="912"/>
-    <row r="913"/>
-    <row r="914"/>
-    <row r="915"/>
-    <row r="916"/>
-    <row r="917"/>
-    <row r="918"/>
-    <row r="919"/>
-    <row r="920"/>
-    <row r="921"/>
-    <row r="922"/>
-    <row r="923"/>
-    <row r="924"/>
-    <row r="925"/>
-    <row r="926"/>
-    <row r="927"/>
-    <row r="928"/>
-    <row r="929"/>
-    <row r="930"/>
-    <row r="931"/>
-    <row r="932"/>
-    <row r="933"/>
-    <row r="934"/>
-    <row r="935"/>
-    <row r="936"/>
-    <row r="937"/>
-    <row r="938"/>
-    <row r="939"/>
-    <row r="940"/>
-    <row r="941"/>
-    <row r="942"/>
-    <row r="943"/>
-    <row r="944"/>
-    <row r="945"/>
-    <row r="946"/>
-    <row r="947"/>
-    <row r="948"/>
-    <row r="949"/>
-    <row r="950"/>
-    <row r="951"/>
-    <row r="952"/>
-    <row r="953"/>
-    <row r="954"/>
-    <row r="955"/>
-    <row r="956"/>
-    <row r="957"/>
-    <row r="958"/>
-    <row r="959"/>
-    <row r="960"/>
-    <row r="961"/>
-    <row r="962"/>
-    <row r="963"/>
-    <row r="964"/>
-    <row r="965"/>
-    <row r="966"/>
-    <row r="967"/>
-    <row r="968"/>
-    <row r="969"/>
-    <row r="970"/>
-    <row r="971"/>
-    <row r="972"/>
-    <row r="973"/>
-    <row r="974"/>
-    <row r="975"/>
-    <row r="976"/>
-    <row r="977"/>
-    <row r="978"/>
-    <row r="979"/>
-    <row r="980"/>
-    <row r="981"/>
-    <row r="982"/>
-    <row r="983"/>
-    <row r="984"/>
-    <row r="985"/>
-    <row r="986"/>
-    <row r="987"/>
-    <row r="988"/>
-    <row r="989"/>
-    <row r="990"/>
-    <row r="991"/>
-    <row r="992"/>
-    <row r="993"/>
-    <row r="994"/>
-    <row r="995"/>
-    <row r="996"/>
-    <row r="997"/>
-    <row r="998"/>
-    <row r="999"/>
-    <row r="1000"/>
+    <row r="83" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="84" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="85" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="86" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="87" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="88" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="89" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="90" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="91" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="92" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="93" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="94" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="95" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="96" spans="1:16" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="$A$1:$P$82"/>
+  <autoFilter ref="A1:P82" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="5">
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="E52:F52"/>
@@ -3906,25 +4107,24 @@
     <mergeCell ref="E77:F77"/>
     <mergeCell ref="E80:F80"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>110</v>
       </c>
@@ -3938,79 +4138,79 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D2" s="15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="15">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="15">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="15">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="12">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="12">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D7" s="12">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IN-719 crec table defs (#54)
* generate the complicated crec conditions
order the table defs

* missed the extra fields

* order the table defs
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B85872-7F01-5C45-8BF9-5E71D828171E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF15AAD-9051-D244-AAF7-815DC5EFE8BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="130">
   <si>
     <t>table_name</t>
   </si>
@@ -496,6 +496,13 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp = {"date": "Modify", "time": "at.1"} 
+latest = {"col": "timestamp", "per": "Case"}</t>
+  </si>
+  <si>
+    <t>Modify, at.1, Case</t>
   </si>
 </sst>
 </file>
@@ -619,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -650,10 +657,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,56 +881,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC95F4-02E8-0A4B-AAFA-EC43C582E824}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="49.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:8" s="19" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="D2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>125</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2367,8 +2386,8 @@
       <c r="D50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="19"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -2423,8 +2442,8 @@
       <c r="D52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="19"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -3067,8 +3086,8 @@
       <c r="D75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="19"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="22"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -3125,8 +3144,8 @@
       <c r="D77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="19"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="22"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -3215,8 +3234,8 @@
       <c r="D80" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="E80" s="18"/>
-      <c r="F80" s="19"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="22"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>

</xml_diff>

<commit_message>
IN-957 Use "at" instead of "at.1" for crec (#79)
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2E40A-55DB-F040-A3D6-7813E8B9AEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F2FB4-92C1-D94F-A088-5444CBA8895C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="4340" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="3" r:id="rId1"/>
@@ -479,11 +479,11 @@
     <t>data</t>
   </si>
   <si>
-    <t>convert_to_timestamp = {"date": "Modify", "time": "at.1"} 
+    <t>Modify, at1, Case</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp = {"date": "Modify", "time": "at1"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
-  </si>
-  <si>
-    <t>Modify, at.1, Case</t>
   </si>
 </sst>
 </file>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC95F4-02E8-0A4B-AAFA-EC43C582E824}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -897,10 +897,10 @@
         <v>119</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -915,8 +915,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IN-957 Use "at" instead of "at.1" for crec (#80)
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F2FB4-92C1-D94F-A088-5444CBA8895C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC07027-D862-994D-906A-80371D58D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,10 +479,10 @@
     <t>data</t>
   </si>
   <si>
-    <t>Modify, at1, Case</t>
-  </si>
-  <si>
-    <t>convert_to_timestamp = {"date": "Modify", "time": "at1"} 
+    <t>Modify, at, Case</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp = {"date": "Modify", "time": "at"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
   </si>
 </sst>
@@ -843,7 +843,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
IN-940 Add mappings for fee reductions; Fix a small bug in Crec mapping (#94)
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Crec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC07027-D862-994D-906A-80371D58D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977B1F0-BA1D-3B45-86AE-7EE99BE72EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,9 +473,6 @@
     <t>crec</t>
   </si>
   <si>
-    <t>client</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   <si>
     <t>convert_to_timestamp = {"date": "Modify", "time": "at"} 
 latest = {"col": "timestamp", "per": "Case"}</t>
+  </si>
+  <si>
+    <t>clients</t>
   </si>
 </sst>
 </file>
@@ -843,7 +843,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -885,22 +885,22 @@
         <v>119</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>119</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>